<commit_message>
Merged PR 53208: Added TC [252668]
Added TC [252668]

Related work items: #252668, #534745, #534801, #534806
</commit_message>
<xml_diff>
--- a/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DVV/LoginData.xlsx
+++ b/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DVV/LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\EnterpriseUX.Automation\West.EnterpriseUX.Automation\MobileAutomationCrossPlatform\TestData\DVV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DVV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961E1DFC-B8B1-4C6B-81B4-6AE9196571ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3045B046-4DD3-4A63-9573-498AAF89DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>emailId</t>
   </si>
   <si>
-    <t>PRAPPP1@WESTPHARMA.COM</t>
+    <t>Test_UX09@westpharma.com</t>
   </si>
   <si>
-    <t>Testing$2020</t>
+    <t>Westpharm@2019</t>
   </si>
 </sst>
 </file>
@@ -368,13 +368,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -390,15 +390,16 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{23B0AECB-6320-4370-900F-FD3F1F93D1BF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{A0E86AF5-E76D-4DF9-B4DA-2B9BFB788604}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>